<commit_message>
data straightening and poster
</commit_message>
<xml_diff>
--- a/Data/TOPAS Data/Overlap1.xlsx
+++ b/Data/TOPAS Data/Overlap1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlottezehnder/Documents/laserStabilization/Data/TOPAS Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2971A40D-99C0-AA4B-8DF7-5515DA9F61F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C06819-8172-0E4C-85BF-7400DA3C003E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="460" windowWidth="20020" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Piezo Voltage (V)</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Frequency Change</t>
+  </si>
+  <si>
+    <t>=</t>
   </si>
 </sst>
 </file>
@@ -34252,10 +34255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1018"/>
+  <dimension ref="A1:O1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H17" zoomScale="169" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35007,7 +35010,7 @@
         <v>7.1651718520716889E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>50.581023999999999</v>
       </c>
@@ -35030,7 +35033,7 @@
         <v>7.1709673915389127E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>50.606650999999999</v>
       </c>
@@ -35053,7 +35056,7 @@
         <v>-6.0533827948482111E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>50.632305000000002</v>
       </c>
@@ -35076,7 +35079,7 @@
         <v>-9.7604930985538407E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>50.657927999999998</v>
       </c>
@@ -35099,7 +35102,7 @@
         <v>-1.7146820181300482E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>50.683582000000001</v>
       </c>
@@ -35122,7 +35125,7 @@
         <v>1.3839866668054202E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>50.709229000000001</v>
       </c>
@@ -35145,7 +35148,7 @@
         <v>-8.742149168946417E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>50.734862999999997</v>
       </c>
@@ -35168,7 +35171,7 @@
         <v>-9.1996001728843202E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>50.760497999999998</v>
       </c>
@@ -35191,7 +35194,7 @@
         <v>4.792460983279595E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>50.786140000000003</v>
       </c>
@@ -35214,7 +35217,7 @@
         <v>1.0445966886605401E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>50.811774999999997</v>
       </c>
@@ -35237,7 +35240,7 @@
         <v>-4.4355099523395169E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>50.837420999999999</v>
       </c>
@@ -35260,7 +35263,7 @@
         <v>-1.4925622980487135E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>50.863075000000002</v>
       </c>
@@ -35283,7 +35286,7 @@
         <v>-5.7830257457634759E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>50.888699000000003</v>
       </c>
@@ -35306,7 +35309,7 @@
         <v>1.2145983235457708E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>50.914352000000001</v>
       </c>
@@ -35328,8 +35331,11 @@
         <f t="shared" si="2"/>
         <v>6.1350578140574596E-4</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="O46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>50.940005999999997</v>
       </c>
@@ -35352,7 +35358,7 @@
         <v>-8.5027661838697755E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>50.965632999999997</v>
       </c>

</xml_diff>